<commit_message>
Update to push US data
</commit_message>
<xml_diff>
--- a/data-raw/counts_all/counts_all.xlsx
+++ b/data-raw/counts_all/counts_all.xlsx
@@ -405,7 +405,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -429,7 +429,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -525,7 +525,7 @@
         <v>6</v>
       </c>
       <c r="E7">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -549,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -573,7 +573,7 @@
         <v>8</v>
       </c>
       <c r="E9">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -597,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -621,7 +621,7 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -645,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="E12">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -669,7 +669,7 @@
         <v>12</v>
       </c>
       <c r="E13">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -765,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="E17">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -789,7 +789,7 @@
         <v>17</v>
       </c>
       <c r="E18">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -813,7 +813,7 @@
         <v>18</v>
       </c>
       <c r="E19">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
         <v>19</v>
       </c>
       <c r="E20">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -885,7 +885,7 @@
         <v>21</v>
       </c>
       <c r="E22">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -909,7 +909,7 @@
         <v>22</v>
       </c>
       <c r="E23">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -957,7 +957,7 @@
         <v>24</v>
       </c>
       <c r="E25">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -981,7 +981,7 @@
         <v>25</v>
       </c>
       <c r="E26">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
         <v>26</v>
       </c>
       <c r="E27">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1029,7 +1029,7 @@
         <v>27</v>
       </c>
       <c r="E28">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1077,7 +1077,7 @@
         <v>29</v>
       </c>
       <c r="E30">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
         <v>30</v>
       </c>
       <c r="E31">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1125,7 +1125,7 @@
         <v>31</v>
       </c>
       <c r="E32">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1149,7 +1149,7 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
         <v>33</v>
       </c>
       <c r="E34">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
         <v>34</v>
       </c>
       <c r="E35">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1245,7 +1245,7 @@
         <v>36</v>
       </c>
       <c r="E37">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1317,7 +1317,7 @@
         <v>39</v>
       </c>
       <c r="E40">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1365,7 +1365,7 @@
         <v>41</v>
       </c>
       <c r="E42">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1389,7 +1389,7 @@
         <v>42</v>
       </c>
       <c r="E43">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1413,7 +1413,7 @@
         <v>43</v>
       </c>
       <c r="E44">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1461,7 +1461,7 @@
         <v>45</v>
       </c>
       <c r="E46">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -1557,7 +1557,7 @@
         <v>49</v>
       </c>
       <c r="E50">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -1581,7 +1581,7 @@
         <v>50</v>
       </c>
       <c r="E51">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -1605,7 +1605,7 @@
         <v>51</v>
       </c>
       <c r="E52">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
         <v>53</v>
       </c>
       <c r="E54">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -1677,7 +1677,7 @@
         <v>54</v>
       </c>
       <c r="E55">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -1701,7 +1701,7 @@
         <v>55</v>
       </c>
       <c r="E56">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -1725,7 +1725,7 @@
         <v>56</v>
       </c>
       <c r="E57">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -1749,7 +1749,7 @@
         <v>57</v>
       </c>
       <c r="E58">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -1797,7 +1797,7 @@
         <v>59</v>
       </c>
       <c r="E60">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -1821,7 +1821,7 @@
         <v>60</v>
       </c>
       <c r="E61">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -1845,7 +1845,7 @@
         <v>61</v>
       </c>
       <c r="E62">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -1917,7 +1917,7 @@
         <v>64</v>
       </c>
       <c r="E65">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -1965,7 +1965,7 @@
         <v>66</v>
       </c>
       <c r="E67">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
         <v>68</v>
       </c>
       <c r="E69">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -2037,7 +2037,7 @@
         <v>69</v>
       </c>
       <c r="E70">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -2061,7 +2061,7 @@
         <v>70</v>
       </c>
       <c r="E71">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -2085,7 +2085,7 @@
         <v>71</v>
       </c>
       <c r="E72">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -2109,7 +2109,7 @@
         <v>72</v>
       </c>
       <c r="E73">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -2133,7 +2133,7 @@
         <v>73</v>
       </c>
       <c r="E74">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -2181,7 +2181,7 @@
         <v>75</v>
       </c>
       <c r="E76">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -2205,7 +2205,7 @@
         <v>76</v>
       </c>
       <c r="E77">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -2253,7 +2253,7 @@
         <v>78</v>
       </c>
       <c r="E79">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -2277,7 +2277,7 @@
         <v>79</v>
       </c>
       <c r="E80">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -2373,7 +2373,7 @@
         <v>83</v>
       </c>
       <c r="E84">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -2397,7 +2397,7 @@
         <v>84</v>
       </c>
       <c r="E85">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -2421,7 +2421,7 @@
         <v>85</v>
       </c>
       <c r="E86">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -2445,7 +2445,7 @@
         <v>86</v>
       </c>
       <c r="E87">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -2469,7 +2469,7 @@
         <v>87</v>
       </c>
       <c r="E88">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -2493,7 +2493,7 @@
         <v>88</v>
       </c>
       <c r="E89">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -2541,7 +2541,7 @@
         <v>90</v>
       </c>
       <c r="E91">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -2565,7 +2565,7 @@
         <v>91</v>
       </c>
       <c r="E92">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -2589,7 +2589,7 @@
         <v>92</v>
       </c>
       <c r="E93">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -2613,7 +2613,7 @@
         <v>93</v>
       </c>
       <c r="E94">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -2637,7 +2637,7 @@
         <v>94</v>
       </c>
       <c r="E95">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -2661,7 +2661,7 @@
         <v>95</v>
       </c>
       <c r="E96">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -2733,7 +2733,7 @@
         <v>98</v>
       </c>
       <c r="E99">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -2757,7 +2757,7 @@
         <v>99</v>
       </c>
       <c r="E100">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -2781,7 +2781,7 @@
         <v>100</v>
       </c>
       <c r="E101">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -2829,7 +2829,7 @@
         <v>102</v>
       </c>
       <c r="E103">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
         <v>103</v>
       </c>
       <c r="E104">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -2877,7 +2877,7 @@
         <v>104</v>
       </c>
       <c r="E105">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -2901,7 +2901,7 @@
         <v>105</v>
       </c>
       <c r="E106">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -2925,7 +2925,7 @@
         <v>106</v>
       </c>
       <c r="E107">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
@@ -2997,7 +2997,7 @@
         <v>109</v>
       </c>
       <c r="E110">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -3021,7 +3021,7 @@
         <v>110</v>
       </c>
       <c r="E111">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -3045,7 +3045,7 @@
         <v>111</v>
       </c>
       <c r="E112">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -3069,7 +3069,7 @@
         <v>112</v>
       </c>
       <c r="E113">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -3093,7 +3093,7 @@
         <v>113</v>
       </c>
       <c r="E114">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -3117,7 +3117,7 @@
         <v>114</v>
       </c>
       <c r="E115">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -3141,7 +3141,7 @@
         <v>115</v>
       </c>
       <c r="E116">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -3165,7 +3165,7 @@
         <v>116</v>
       </c>
       <c r="E117">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
@@ -3189,7 +3189,7 @@
         <v>117</v>
       </c>
       <c r="E118">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
@@ -3237,7 +3237,7 @@
         <v>119</v>
       </c>
       <c r="E120">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -3261,7 +3261,7 @@
         <v>120</v>
       </c>
       <c r="E121">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -3285,7 +3285,7 @@
         <v>121</v>
       </c>
       <c r="E122">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
@@ -3381,7 +3381,7 @@
         <v>125</v>
       </c>
       <c r="E126">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
@@ -3429,7 +3429,7 @@
         <v>127</v>
       </c>
       <c r="E128">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -3453,7 +3453,7 @@
         <v>128</v>
       </c>
       <c r="E129">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
@@ -3477,7 +3477,7 @@
         <v>129</v>
       </c>
       <c r="E130">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
@@ -3549,7 +3549,7 @@
         <v>132</v>
       </c>
       <c r="E133">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
@@ -3573,7 +3573,7 @@
         <v>133</v>
       </c>
       <c r="E134">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -3597,7 +3597,7 @@
         <v>134</v>
       </c>
       <c r="E135">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>136</v>
       </c>
       <c r="E137">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -3669,7 +3669,7 @@
         <v>137</v>
       </c>
       <c r="E138">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -3693,7 +3693,7 @@
         <v>138</v>
       </c>
       <c r="E139">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -3741,7 +3741,7 @@
         <v>140</v>
       </c>
       <c r="E141">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
@@ -3765,7 +3765,7 @@
         <v>141</v>
       </c>
       <c r="E142">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -3789,7 +3789,7 @@
         <v>142</v>
       </c>
       <c r="E143">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
@@ -3813,7 +3813,7 @@
         <v>143</v>
       </c>
       <c r="E144">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
         <v>144</v>
       </c>
       <c r="E145">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F145" t="inlineStr">
         <is>
@@ -3861,7 +3861,7 @@
         <v>145</v>
       </c>
       <c r="E146">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -3885,7 +3885,7 @@
         <v>146</v>
       </c>
       <c r="E147">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -3957,7 +3957,7 @@
         <v>149</v>
       </c>
       <c r="E150">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
@@ -3981,7 +3981,7 @@
         <v>150</v>
       </c>
       <c r="E151">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
@@ -4005,7 +4005,7 @@
         <v>151</v>
       </c>
       <c r="E152">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -4029,7 +4029,7 @@
         <v>152</v>
       </c>
       <c r="E153">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
@@ -4053,7 +4053,7 @@
         <v>153</v>
       </c>
       <c r="E154">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
@@ -4077,7 +4077,7 @@
         <v>154</v>
       </c>
       <c r="E155">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
@@ -4125,7 +4125,7 @@
         <v>156</v>
       </c>
       <c r="E157">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
@@ -4149,7 +4149,7 @@
         <v>157</v>
       </c>
       <c r="E158">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
@@ -4197,7 +4197,7 @@
         <v>159</v>
       </c>
       <c r="E160">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F160" t="inlineStr">
         <is>
@@ -4245,7 +4245,7 @@
         <v>161</v>
       </c>
       <c r="E162">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
@@ -4269,7 +4269,7 @@
         <v>162</v>
       </c>
       <c r="E163">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F163" t="inlineStr">
         <is>
@@ -4293,7 +4293,7 @@
         <v>163</v>
       </c>
       <c r="E164">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
@@ -4365,7 +4365,7 @@
         <v>166</v>
       </c>
       <c r="E167">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F167" t="inlineStr">
         <is>
@@ -4389,7 +4389,7 @@
         <v>167</v>
       </c>
       <c r="E168">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
@@ -4413,7 +4413,7 @@
         <v>168</v>
       </c>
       <c r="E169">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
@@ -4437,7 +4437,7 @@
         <v>169</v>
       </c>
       <c r="E170">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F170" t="inlineStr">
         <is>
@@ -4461,7 +4461,7 @@
         <v>170</v>
       </c>
       <c r="E171">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F171" t="inlineStr">
         <is>
@@ -4509,7 +4509,7 @@
         <v>172</v>
       </c>
       <c r="E173">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
@@ -4533,7 +4533,7 @@
         <v>173</v>
       </c>
       <c r="E174">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F174" t="inlineStr">
         <is>
@@ -4557,7 +4557,7 @@
         <v>174</v>
       </c>
       <c r="E175">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -4581,7 +4581,7 @@
         <v>175</v>
       </c>
       <c r="E176">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F176" t="inlineStr">
         <is>
@@ -4605,7 +4605,7 @@
         <v>176</v>
       </c>
       <c r="E177">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F177" t="inlineStr">
         <is>
@@ -4629,7 +4629,7 @@
         <v>177</v>
       </c>
       <c r="E178">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -4653,7 +4653,7 @@
         <v>178</v>
       </c>
       <c r="E179">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F179" t="inlineStr">
         <is>
@@ -4725,7 +4725,7 @@
         <v>181</v>
       </c>
       <c r="E182">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -4773,7 +4773,7 @@
         <v>183</v>
       </c>
       <c r="E184">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F184" t="inlineStr">
         <is>
@@ -4797,7 +4797,7 @@
         <v>184</v>
       </c>
       <c r="E185">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
@@ -4821,7 +4821,7 @@
         <v>185</v>
       </c>
       <c r="E186">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -4845,7 +4845,7 @@
         <v>186</v>
       </c>
       <c r="E187">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F187" t="inlineStr">
         <is>
@@ -4869,7 +4869,7 @@
         <v>187</v>
       </c>
       <c r="E188">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -4893,7 +4893,7 @@
         <v>188</v>
       </c>
       <c r="E189">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
@@ -4917,7 +4917,7 @@
         <v>189</v>
       </c>
       <c r="E190">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F190" t="inlineStr">
         <is>
@@ -4989,7 +4989,7 @@
         <v>192</v>
       </c>
       <c r="E193">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -5013,7 +5013,7 @@
         <v>193</v>
       </c>
       <c r="E194">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
@@ -5061,7 +5061,7 @@
         <v>195</v>
       </c>
       <c r="E196">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F196" t="inlineStr">
         <is>
@@ -5109,7 +5109,7 @@
         <v>197</v>
       </c>
       <c r="E198">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
@@ -5133,7 +5133,7 @@
         <v>198</v>
       </c>
       <c r="E199">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
@@ -5157,7 +5157,7 @@
         <v>199</v>
       </c>
       <c r="E200">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F200" t="inlineStr">
         <is>
@@ -5181,7 +5181,7 @@
         <v>200</v>
       </c>
       <c r="E201">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -5205,7 +5205,7 @@
         <v>201</v>
       </c>
       <c r="E202">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F202" t="inlineStr">
         <is>
@@ -5229,7 +5229,7 @@
         <v>202</v>
       </c>
       <c r="E203">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F203" t="inlineStr">
         <is>
@@ -5277,7 +5277,7 @@
         <v>204</v>
       </c>
       <c r="E205">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -5325,7 +5325,7 @@
         <v>206</v>
       </c>
       <c r="E207">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
@@ -5349,7 +5349,7 @@
         <v>207</v>
       </c>
       <c r="E208">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F208" t="inlineStr">
         <is>
@@ -5373,7 +5373,7 @@
         <v>208</v>
       </c>
       <c r="E209">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F209" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
         <v>209</v>
       </c>
       <c r="E210">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F210" t="inlineStr">
         <is>
@@ -5421,7 +5421,7 @@
         <v>210</v>
       </c>
       <c r="E211">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -5445,7 +5445,7 @@
         <v>211</v>
       </c>
       <c r="E212">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F212" t="inlineStr">
         <is>
@@ -5469,7 +5469,7 @@
         <v>212</v>
       </c>
       <c r="E213">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F213" t="inlineStr">
         <is>
@@ -5493,7 +5493,7 @@
         <v>213</v>
       </c>
       <c r="E214">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F214" t="inlineStr">
         <is>
@@ -5517,7 +5517,7 @@
         <v>214</v>
       </c>
       <c r="E215">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F215" t="inlineStr">
         <is>
@@ -5541,7 +5541,7 @@
         <v>215</v>
       </c>
       <c r="E216">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F216" t="inlineStr">
         <is>
@@ -5589,7 +5589,7 @@
         <v>217</v>
       </c>
       <c r="E218">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F218" t="inlineStr">
         <is>
@@ -5613,7 +5613,7 @@
         <v>218</v>
       </c>
       <c r="E219">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F219" t="inlineStr">
         <is>
@@ -5637,7 +5637,7 @@
         <v>219</v>
       </c>
       <c r="E220">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F220" t="inlineStr">
         <is>
@@ -5661,7 +5661,7 @@
         <v>220</v>
       </c>
       <c r="E221">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F221" t="inlineStr">
         <is>
@@ -5685,7 +5685,7 @@
         <v>221</v>
       </c>
       <c r="E222">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F222" t="inlineStr">
         <is>
@@ -5709,7 +5709,7 @@
         <v>222</v>
       </c>
       <c r="E223">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F223" t="inlineStr">
         <is>
@@ -5733,7 +5733,7 @@
         <v>223</v>
       </c>
       <c r="E224">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F224" t="inlineStr">
         <is>
@@ -5757,7 +5757,7 @@
         <v>224</v>
       </c>
       <c r="E225">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F225" t="inlineStr">
         <is>
@@ -5781,7 +5781,7 @@
         <v>225</v>
       </c>
       <c r="E226">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F226" t="inlineStr">
         <is>
@@ -5805,7 +5805,7 @@
         <v>226</v>
       </c>
       <c r="E227">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F227" t="inlineStr">
         <is>
@@ -5829,7 +5829,7 @@
         <v>227</v>
       </c>
       <c r="E228">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F228" t="inlineStr">
         <is>
@@ -5853,7 +5853,7 @@
         <v>228</v>
       </c>
       <c r="E229">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F229" t="inlineStr">
         <is>
@@ -5877,7 +5877,7 @@
         <v>229</v>
       </c>
       <c r="E230">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F230" t="inlineStr">
         <is>
@@ -5901,7 +5901,7 @@
         <v>230</v>
       </c>
       <c r="E231">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F231" t="inlineStr">
         <is>
@@ -5949,7 +5949,7 @@
         <v>232</v>
       </c>
       <c r="E233">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F233" t="inlineStr">
         <is>
@@ -5973,7 +5973,7 @@
         <v>233</v>
       </c>
       <c r="E234">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F234" t="inlineStr">
         <is>
@@ -5997,7 +5997,7 @@
         <v>234</v>
       </c>
       <c r="E235">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F235" t="inlineStr">
         <is>
@@ -6021,7 +6021,7 @@
         <v>235</v>
       </c>
       <c r="E236">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F236" t="inlineStr">
         <is>
@@ -6045,7 +6045,7 @@
         <v>236</v>
       </c>
       <c r="E237">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F237" t="inlineStr">
         <is>
@@ -6069,7 +6069,7 @@
         <v>237</v>
       </c>
       <c r="E238">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F238" t="inlineStr">
         <is>
@@ -6093,7 +6093,7 @@
         <v>238</v>
       </c>
       <c r="E239">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F239" t="inlineStr">
         <is>
@@ -6117,7 +6117,7 @@
         <v>239</v>
       </c>
       <c r="E240">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F240" t="inlineStr">
         <is>
@@ -6141,7 +6141,7 @@
         <v>240</v>
       </c>
       <c r="E241">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F241" t="inlineStr">
         <is>
@@ -6213,7 +6213,7 @@
         <v>243</v>
       </c>
       <c r="E244">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F244" t="inlineStr">
         <is>
@@ -6237,7 +6237,7 @@
         <v>244</v>
       </c>
       <c r="E245">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F245" t="inlineStr">
         <is>
@@ -6261,7 +6261,7 @@
         <v>245</v>
       </c>
       <c r="E246">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F246" t="inlineStr">
         <is>
@@ -6285,7 +6285,7 @@
         <v>246</v>
       </c>
       <c r="E247">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F247" t="inlineStr">
         <is>
@@ -6309,7 +6309,7 @@
         <v>247</v>
       </c>
       <c r="E248">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F248" t="inlineStr">
         <is>
@@ -6333,7 +6333,7 @@
         <v>248</v>
       </c>
       <c r="E249">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F249" t="inlineStr">
         <is>
@@ -6357,7 +6357,7 @@
         <v>249</v>
       </c>
       <c r="E250">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F250" t="inlineStr">
         <is>
@@ -6381,7 +6381,7 @@
         <v>250</v>
       </c>
       <c r="E251">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F251" t="inlineStr">
         <is>
@@ -6405,7 +6405,7 @@
         <v>251</v>
       </c>
       <c r="E252">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F252" t="inlineStr">
         <is>
@@ -6453,7 +6453,7 @@
         <v>253</v>
       </c>
       <c r="E254">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F254" t="inlineStr">
         <is>
@@ -6477,7 +6477,7 @@
         <v>254</v>
       </c>
       <c r="E255">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F255" t="inlineStr">
         <is>
@@ -6501,7 +6501,7 @@
         <v>255</v>
       </c>
       <c r="E256">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F256" t="inlineStr">
         <is>
@@ -6549,7 +6549,7 @@
         <v>257</v>
       </c>
       <c r="E258">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F258" t="inlineStr">
         <is>
@@ -6573,7 +6573,7 @@
         <v>258</v>
       </c>
       <c r="E259">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F259" t="inlineStr">
         <is>
@@ -6597,7 +6597,7 @@
         <v>259</v>
       </c>
       <c r="E260">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F260" t="inlineStr">
         <is>
@@ -6621,7 +6621,7 @@
         <v>260</v>
       </c>
       <c r="E261">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F261" t="inlineStr">
         <is>
@@ -6645,7 +6645,7 @@
         <v>261</v>
       </c>
       <c r="E262">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F262" t="inlineStr">
         <is>
@@ -6669,7 +6669,7 @@
         <v>262</v>
       </c>
       <c r="E263">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F263" t="inlineStr">
         <is>
@@ -6693,7 +6693,7 @@
         <v>263</v>
       </c>
       <c r="E264">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F264" t="inlineStr">
         <is>
@@ -6717,7 +6717,7 @@
         <v>264</v>
       </c>
       <c r="E265">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F265" t="inlineStr">
         <is>
@@ -6789,7 +6789,7 @@
         <v>267</v>
       </c>
       <c r="E268">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F268" t="inlineStr">
         <is>
@@ -6837,7 +6837,7 @@
         <v>269</v>
       </c>
       <c r="E270">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F270" t="inlineStr">
         <is>
@@ -6861,7 +6861,7 @@
         <v>270</v>
       </c>
       <c r="E271">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F271" t="inlineStr">
         <is>
@@ -6885,7 +6885,7 @@
         <v>271</v>
       </c>
       <c r="E272">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F272" t="inlineStr">
         <is>
@@ -6909,7 +6909,7 @@
         <v>272</v>
       </c>
       <c r="E273">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F273" t="inlineStr">
         <is>
@@ -6957,7 +6957,7 @@
         <v>274</v>
       </c>
       <c r="E275">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F275" t="inlineStr">
         <is>
@@ -6981,7 +6981,7 @@
         <v>275</v>
       </c>
       <c r="E276">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F276" t="inlineStr">
         <is>
@@ -7029,7 +7029,7 @@
         <v>277</v>
       </c>
       <c r="E278">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F278" t="inlineStr">
         <is>
@@ -7077,7 +7077,7 @@
         <v>279</v>
       </c>
       <c r="E280">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F280" t="inlineStr">
         <is>
@@ -7101,7 +7101,7 @@
         <v>280</v>
       </c>
       <c r="E281">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F281" t="inlineStr">
         <is>
@@ -7149,7 +7149,7 @@
         <v>282</v>
       </c>
       <c r="E283">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F283" t="inlineStr">
         <is>
@@ -7197,7 +7197,7 @@
         <v>284</v>
       </c>
       <c r="E285">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F285" t="inlineStr">
         <is>
@@ -7221,7 +7221,7 @@
         <v>285</v>
       </c>
       <c r="E286">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F286" t="inlineStr">
         <is>
@@ -7245,7 +7245,7 @@
         <v>286</v>
       </c>
       <c r="E287">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F287" t="inlineStr">
         <is>
@@ -7269,7 +7269,7 @@
         <v>287</v>
       </c>
       <c r="E288">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F288" t="inlineStr">
         <is>
@@ -7293,7 +7293,7 @@
         <v>288</v>
       </c>
       <c r="E289">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F289" t="inlineStr">
         <is>
@@ -7317,7 +7317,7 @@
         <v>289</v>
       </c>
       <c r="E290">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F290" t="inlineStr">
         <is>
@@ -7341,7 +7341,7 @@
         <v>290</v>
       </c>
       <c r="E291">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F291" t="inlineStr">
         <is>
@@ -7413,7 +7413,7 @@
         <v>293</v>
       </c>
       <c r="E294">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F294" t="inlineStr">
         <is>
@@ -7461,7 +7461,7 @@
         <v>295</v>
       </c>
       <c r="E296">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F296" t="inlineStr">
         <is>
@@ -7485,7 +7485,7 @@
         <v>296</v>
       </c>
       <c r="E297">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F297" t="inlineStr">
         <is>
@@ -7509,7 +7509,7 @@
         <v>297</v>
       </c>
       <c r="E298">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F298" t="inlineStr">
         <is>
@@ -7533,7 +7533,7 @@
         <v>298</v>
       </c>
       <c r="E299">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
@@ -7581,7 +7581,7 @@
         <v>300</v>
       </c>
       <c r="E301">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F301" t="inlineStr">
         <is>
@@ -7605,7 +7605,7 @@
         <v>301</v>
       </c>
       <c r="E302">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F302" t="inlineStr">
         <is>
@@ -7629,7 +7629,7 @@
         <v>302</v>
       </c>
       <c r="E303">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F303" t="inlineStr">
         <is>
@@ -7677,7 +7677,7 @@
         <v>304</v>
       </c>
       <c r="E305">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F305" t="inlineStr">
         <is>
@@ -7773,7 +7773,7 @@
         <v>308</v>
       </c>
       <c r="E309">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F309" t="inlineStr">
         <is>
@@ -7821,7 +7821,7 @@
         <v>310</v>
       </c>
       <c r="E311">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F311" t="inlineStr">
         <is>
@@ -7845,7 +7845,7 @@
         <v>311</v>
       </c>
       <c r="E312">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F312" t="inlineStr">
         <is>
@@ -7869,7 +7869,7 @@
         <v>312</v>
       </c>
       <c r="E313">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F313" t="inlineStr">
         <is>
@@ -7893,7 +7893,7 @@
         <v>313</v>
       </c>
       <c r="E314">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F314" t="inlineStr">
         <is>
@@ -7941,7 +7941,7 @@
         <v>315</v>
       </c>
       <c r="E316">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F316" t="inlineStr">
         <is>
@@ -7965,7 +7965,7 @@
         <v>316</v>
       </c>
       <c r="E317">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F317" t="inlineStr">
         <is>
@@ -7989,7 +7989,7 @@
         <v>317</v>
       </c>
       <c r="E318">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F318" t="inlineStr">
         <is>
@@ -8013,7 +8013,7 @@
         <v>318</v>
       </c>
       <c r="E319">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F319" t="inlineStr">
         <is>
@@ -8037,7 +8037,7 @@
         <v>319</v>
       </c>
       <c r="E320">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F320" t="inlineStr">
         <is>
@@ -8061,7 +8061,7 @@
         <v>320</v>
       </c>
       <c r="E321">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F321" t="inlineStr">
         <is>
@@ -8109,7 +8109,7 @@
         <v>322</v>
       </c>
       <c r="E323">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F323" t="inlineStr">
         <is>
@@ -8157,7 +8157,7 @@
         <v>324</v>
       </c>
       <c r="E325">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F325" t="inlineStr">
         <is>
@@ -8181,7 +8181,7 @@
         <v>325</v>
       </c>
       <c r="E326">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F326" t="inlineStr">
         <is>
@@ -8205,7 +8205,7 @@
         <v>326</v>
       </c>
       <c r="E327">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F327" t="inlineStr">
         <is>
@@ -8229,7 +8229,7 @@
         <v>327</v>
       </c>
       <c r="E328">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F328" t="inlineStr">
         <is>
@@ -8277,7 +8277,7 @@
         <v>329</v>
       </c>
       <c r="E330">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F330" t="inlineStr">
         <is>
@@ -8349,7 +8349,7 @@
         <v>332</v>
       </c>
       <c r="E333">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F333" t="inlineStr">
         <is>
@@ -8373,7 +8373,7 @@
         <v>333</v>
       </c>
       <c r="E334">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F334" t="inlineStr">
         <is>
@@ -8397,7 +8397,7 @@
         <v>334</v>
       </c>
       <c r="E335">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F335" t="inlineStr">
         <is>
@@ -8445,7 +8445,7 @@
         <v>336</v>
       </c>
       <c r="E337">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F337" t="inlineStr">
         <is>
@@ -8469,7 +8469,7 @@
         <v>337</v>
       </c>
       <c r="E338">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F338" t="inlineStr">
         <is>
@@ -8493,7 +8493,7 @@
         <v>338</v>
       </c>
       <c r="E339">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F339" t="inlineStr">
         <is>
@@ -8517,7 +8517,7 @@
         <v>339</v>
       </c>
       <c r="E340">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F340" t="inlineStr">
         <is>
@@ -8541,7 +8541,7 @@
         <v>340</v>
       </c>
       <c r="E341">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F341" t="inlineStr">
         <is>
@@ -8565,7 +8565,7 @@
         <v>341</v>
       </c>
       <c r="E342">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F342" t="inlineStr">
         <is>
@@ -8589,7 +8589,7 @@
         <v>342</v>
       </c>
       <c r="E343">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F343" t="inlineStr">
         <is>
@@ -8637,7 +8637,7 @@
         <v>344</v>
       </c>
       <c r="E345">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F345" t="inlineStr">
         <is>
@@ -8661,7 +8661,7 @@
         <v>345</v>
       </c>
       <c r="E346">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F346" t="inlineStr">
         <is>
@@ -8685,7 +8685,7 @@
         <v>346</v>
       </c>
       <c r="E347">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F347" t="inlineStr">
         <is>
@@ -8805,7 +8805,7 @@
         <v>351</v>
       </c>
       <c r="E352">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F352" t="inlineStr">
         <is>
@@ -8829,7 +8829,7 @@
         <v>352</v>
       </c>
       <c r="E353">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F353" t="inlineStr">
         <is>
@@ -8853,7 +8853,7 @@
         <v>353</v>
       </c>
       <c r="E354">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F354" t="inlineStr">
         <is>
@@ -8901,7 +8901,7 @@
         <v>355</v>
       </c>
       <c r="E356">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F356" t="inlineStr">
         <is>
@@ -8925,7 +8925,7 @@
         <v>356</v>
       </c>
       <c r="E357">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F357" t="inlineStr">
         <is>
@@ -8949,7 +8949,7 @@
         <v>357</v>
       </c>
       <c r="E358">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F358" t="inlineStr">
         <is>
@@ -8973,7 +8973,7 @@
         <v>358</v>
       </c>
       <c r="E359">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F359" t="inlineStr">
         <is>
@@ -8997,7 +8997,7 @@
         <v>359</v>
       </c>
       <c r="E360">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F360" t="inlineStr">
         <is>
@@ -9021,7 +9021,7 @@
         <v>360</v>
       </c>
       <c r="E361">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F361" t="inlineStr">
         <is>
@@ -9045,7 +9045,7 @@
         <v>361</v>
       </c>
       <c r="E362">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F362" t="inlineStr">
         <is>
@@ -9069,7 +9069,7 @@
         <v>362</v>
       </c>
       <c r="E363">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F363" t="inlineStr">
         <is>
@@ -9093,7 +9093,7 @@
         <v>363</v>
       </c>
       <c r="E364">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F364" t="inlineStr">
         <is>
@@ -9117,7 +9117,7 @@
         <v>364</v>
       </c>
       <c r="E365">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F365" t="inlineStr">
         <is>
@@ -9141,7 +9141,7 @@
         <v>365</v>
       </c>
       <c r="E366">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F366" t="inlineStr">
         <is>
@@ -9165,7 +9165,7 @@
         <v>366</v>
       </c>
       <c r="E367">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F367" t="inlineStr">
         <is>
@@ -9178,7 +9178,7 @@
         <v>367</v>
       </c>
       <c r="E368">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F368" t="inlineStr">
         <is>
@@ -9202,7 +9202,7 @@
         <v>1</v>
       </c>
       <c r="E369">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F369" t="inlineStr">
         <is>
@@ -9370,7 +9370,7 @@
         <v>8</v>
       </c>
       <c r="E376">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F376" t="inlineStr">
         <is>
@@ -9394,7 +9394,7 @@
         <v>9</v>
       </c>
       <c r="E377">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F377" t="inlineStr">
         <is>
@@ -9418,7 +9418,7 @@
         <v>10</v>
       </c>
       <c r="E378">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F378" t="inlineStr">
         <is>
@@ -9442,7 +9442,7 @@
         <v>11</v>
       </c>
       <c r="E379">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F379" t="inlineStr">
         <is>
@@ -9466,7 +9466,7 @@
         <v>12</v>
       </c>
       <c r="E380">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F380" t="inlineStr">
         <is>
@@ -9538,7 +9538,7 @@
         <v>15</v>
       </c>
       <c r="E383">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F383" t="inlineStr">
         <is>
@@ -9562,7 +9562,7 @@
         <v>16</v>
       </c>
       <c r="E384">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F384" t="inlineStr">
         <is>
@@ -9586,7 +9586,7 @@
         <v>17</v>
       </c>
       <c r="E385">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F385" t="inlineStr">
         <is>
@@ -9610,7 +9610,7 @@
         <v>18</v>
       </c>
       <c r="E386">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F386" t="inlineStr">
         <is>
@@ -9682,7 +9682,7 @@
         <v>21</v>
       </c>
       <c r="E389">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F389" t="inlineStr">
         <is>
@@ -9706,7 +9706,7 @@
         <v>22</v>
       </c>
       <c r="E390">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F390" t="inlineStr">
         <is>
@@ -9802,7 +9802,7 @@
         <v>26</v>
       </c>
       <c r="E394">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F394" t="inlineStr">
         <is>
@@ -9826,7 +9826,7 @@
         <v>27</v>
       </c>
       <c r="E395">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F395" t="inlineStr">
         <is>
@@ -9922,7 +9922,7 @@
         <v>31</v>
       </c>
       <c r="E399">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F399" t="inlineStr">
         <is>
@@ -9994,7 +9994,7 @@
         <v>34</v>
       </c>
       <c r="E402">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F402" t="inlineStr">
         <is>
@@ -10066,7 +10066,7 @@
         <v>37</v>
       </c>
       <c r="E405">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F405" t="inlineStr">
         <is>
@@ -10330,7 +10330,7 @@
         <v>48</v>
       </c>
       <c r="E416">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F416" t="inlineStr">
         <is>
@@ -10378,7 +10378,7 @@
         <v>50</v>
       </c>
       <c r="E418">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F418" t="inlineStr">
         <is>
@@ -10426,7 +10426,7 @@
         <v>52</v>
       </c>
       <c r="E420">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F420" t="inlineStr">
         <is>
@@ -10666,7 +10666,7 @@
         <v>62</v>
       </c>
       <c r="E430">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F430" t="inlineStr">
         <is>
@@ -10738,7 +10738,7 @@
         <v>65</v>
       </c>
       <c r="E433">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F433" t="inlineStr">
         <is>
@@ -10786,7 +10786,7 @@
         <v>67</v>
       </c>
       <c r="E435">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F435" t="inlineStr">
         <is>
@@ -10810,7 +10810,7 @@
         <v>68</v>
       </c>
       <c r="E436">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F436" t="inlineStr">
         <is>
@@ -10858,7 +10858,7 @@
         <v>70</v>
       </c>
       <c r="E438">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F438" t="inlineStr">
         <is>
@@ -10906,7 +10906,7 @@
         <v>72</v>
       </c>
       <c r="E440">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F440" t="inlineStr">
         <is>
@@ -10930,7 +10930,7 @@
         <v>73</v>
       </c>
       <c r="E441">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F441" t="inlineStr">
         <is>
@@ -10978,7 +10978,7 @@
         <v>75</v>
       </c>
       <c r="E443">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F443" t="inlineStr">
         <is>
@@ -11122,7 +11122,7 @@
         <v>81</v>
       </c>
       <c r="E449">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F449" t="inlineStr">
         <is>
@@ -11170,7 +11170,7 @@
         <v>83</v>
       </c>
       <c r="E451">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F451" t="inlineStr">
         <is>
@@ -11194,7 +11194,7 @@
         <v>84</v>
       </c>
       <c r="E452">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F452" t="inlineStr">
         <is>
@@ -11266,7 +11266,7 @@
         <v>87</v>
       </c>
       <c r="E455">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F455" t="inlineStr">
         <is>
@@ -11290,7 +11290,7 @@
         <v>88</v>
       </c>
       <c r="E456">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F456" t="inlineStr">
         <is>
@@ -11362,7 +11362,7 @@
         <v>91</v>
       </c>
       <c r="E459">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F459" t="inlineStr">
         <is>
@@ -11410,7 +11410,7 @@
         <v>93</v>
       </c>
       <c r="E461">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F461" t="inlineStr">
         <is>
@@ -11458,7 +11458,7 @@
         <v>95</v>
       </c>
       <c r="E463">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -11482,7 +11482,7 @@
         <v>96</v>
       </c>
       <c r="E464">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F464" t="inlineStr">
         <is>
@@ -11578,7 +11578,7 @@
         <v>100</v>
       </c>
       <c r="E468">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F468" t="inlineStr">
         <is>
@@ -11626,7 +11626,7 @@
         <v>102</v>
       </c>
       <c r="E470">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F470" t="inlineStr">
         <is>
@@ -11650,7 +11650,7 @@
         <v>103</v>
       </c>
       <c r="E471">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F471" t="inlineStr">
         <is>
@@ -11770,7 +11770,7 @@
         <v>108</v>
       </c>
       <c r="E476">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F476" t="inlineStr">
         <is>
@@ -11794,7 +11794,7 @@
         <v>109</v>
       </c>
       <c r="E477">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F477" t="inlineStr">
         <is>
@@ -11818,7 +11818,7 @@
         <v>110</v>
       </c>
       <c r="E478">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F478" t="inlineStr">
         <is>
@@ -11962,7 +11962,7 @@
         <v>116</v>
       </c>
       <c r="E484">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F484" t="inlineStr">
         <is>
@@ -11986,7 +11986,7 @@
         <v>117</v>
       </c>
       <c r="E485">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F485" t="inlineStr">
         <is>
@@ -12034,7 +12034,7 @@
         <v>119</v>
       </c>
       <c r="E487">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -12106,7 +12106,7 @@
         <v>122</v>
       </c>
       <c r="E490">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F490" t="inlineStr">
         <is>
@@ -12226,7 +12226,7 @@
         <v>127</v>
       </c>
       <c r="E495">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F495" t="inlineStr">
         <is>
@@ -12298,7 +12298,7 @@
         <v>130</v>
       </c>
       <c r="E498">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F498" t="inlineStr">
         <is>
@@ -12346,7 +12346,7 @@
         <v>132</v>
       </c>
       <c r="E500">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F500" t="inlineStr">
         <is>
@@ -12370,7 +12370,7 @@
         <v>133</v>
       </c>
       <c r="E501">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F501" t="inlineStr">
         <is>
@@ -12394,7 +12394,7 @@
         <v>134</v>
       </c>
       <c r="E502">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F502" t="inlineStr">
         <is>
@@ -12418,7 +12418,7 @@
         <v>135</v>
       </c>
       <c r="E503">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F503" t="inlineStr">
         <is>
@@ -12490,7 +12490,7 @@
         <v>138</v>
       </c>
       <c r="E506">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F506" t="inlineStr">
         <is>
@@ -12634,7 +12634,7 @@
         <v>144</v>
       </c>
       <c r="E512">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F512" t="inlineStr">
         <is>
@@ -12682,7 +12682,7 @@
         <v>146</v>
       </c>
       <c r="E514">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F514" t="inlineStr">
         <is>
@@ -12706,7 +12706,7 @@
         <v>147</v>
       </c>
       <c r="E515">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F515" t="inlineStr">
         <is>
@@ -12754,7 +12754,7 @@
         <v>149</v>
       </c>
       <c r="E517">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F517" t="inlineStr">
         <is>
@@ -12778,7 +12778,7 @@
         <v>150</v>
       </c>
       <c r="E518">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F518" t="inlineStr">
         <is>
@@ -12922,7 +12922,7 @@
         <v>156</v>
       </c>
       <c r="E524">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F524" t="inlineStr">
         <is>
@@ -13114,7 +13114,7 @@
         <v>164</v>
       </c>
       <c r="E532">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F532" t="inlineStr">
         <is>
@@ -13162,7 +13162,7 @@
         <v>166</v>
       </c>
       <c r="E534">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F534" t="inlineStr">
         <is>
@@ -13258,7 +13258,7 @@
         <v>170</v>
       </c>
       <c r="E538">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F538" t="inlineStr">
         <is>
@@ -13282,7 +13282,7 @@
         <v>171</v>
       </c>
       <c r="E539">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F539" t="inlineStr">
         <is>
@@ -13306,7 +13306,7 @@
         <v>172</v>
       </c>
       <c r="E540">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -13402,7 +13402,7 @@
         <v>176</v>
       </c>
       <c r="E544">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F544" t="inlineStr">
         <is>
@@ -13522,7 +13522,7 @@
         <v>181</v>
       </c>
       <c r="E549">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F549" t="inlineStr">
         <is>
@@ -13546,7 +13546,7 @@
         <v>182</v>
       </c>
       <c r="E550">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F550" t="inlineStr">
         <is>
@@ -13570,7 +13570,7 @@
         <v>183</v>
       </c>
       <c r="E551">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F551" t="inlineStr">
         <is>
@@ -13618,7 +13618,7 @@
         <v>185</v>
       </c>
       <c r="E553">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F553" t="inlineStr">
         <is>
@@ -13642,7 +13642,7 @@
         <v>186</v>
       </c>
       <c r="E554">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F554" t="inlineStr">
         <is>
@@ -13666,7 +13666,7 @@
         <v>187</v>
       </c>
       <c r="E555">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F555" t="inlineStr">
         <is>
@@ -13690,7 +13690,7 @@
         <v>188</v>
       </c>
       <c r="E556">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F556" t="inlineStr">
         <is>
@@ -13714,7 +13714,7 @@
         <v>189</v>
       </c>
       <c r="E557">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -13762,7 +13762,7 @@
         <v>191</v>
       </c>
       <c r="E559">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F559" t="inlineStr">
         <is>
@@ -13810,7 +13810,7 @@
         <v>193</v>
       </c>
       <c r="E561">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F561" t="inlineStr">
         <is>
@@ -13834,7 +13834,7 @@
         <v>194</v>
       </c>
       <c r="E562">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F562" t="inlineStr">
         <is>
@@ -13858,7 +13858,7 @@
         <v>195</v>
       </c>
       <c r="E563">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F563" t="inlineStr">
         <is>
@@ -13882,7 +13882,7 @@
         <v>196</v>
       </c>
       <c r="E564">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F564" t="inlineStr">
         <is>
@@ -13930,7 +13930,7 @@
         <v>198</v>
       </c>
       <c r="E566">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F566" t="inlineStr">
         <is>
@@ -13978,7 +13978,7 @@
         <v>200</v>
       </c>
       <c r="E568">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F568" t="inlineStr">
         <is>
@@ -14170,7 +14170,7 @@
         <v>208</v>
       </c>
       <c r="E576">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F576" t="inlineStr">
         <is>
@@ -14194,7 +14194,7 @@
         <v>209</v>
       </c>
       <c r="E577">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F577" t="inlineStr">
         <is>
@@ -14218,7 +14218,7 @@
         <v>210</v>
       </c>
       <c r="E578">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F578" t="inlineStr">
         <is>
@@ -14266,7 +14266,7 @@
         <v>212</v>
       </c>
       <c r="E580">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F580" t="inlineStr">
         <is>
@@ -14314,7 +14314,7 @@
         <v>214</v>
       </c>
       <c r="E582">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F582" t="inlineStr">
         <is>
@@ -14338,7 +14338,7 @@
         <v>215</v>
       </c>
       <c r="E583">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F583" t="inlineStr">
         <is>
@@ -14362,7 +14362,7 @@
         <v>216</v>
       </c>
       <c r="E584">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F584" t="inlineStr">
         <is>
@@ -14386,7 +14386,7 @@
         <v>217</v>
       </c>
       <c r="E585">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F585" t="inlineStr">
         <is>
@@ -14506,7 +14506,7 @@
         <v>222</v>
       </c>
       <c r="E590">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F590" t="inlineStr">
         <is>
@@ -14554,7 +14554,7 @@
         <v>224</v>
       </c>
       <c r="E592">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F592" t="inlineStr">
         <is>
@@ -14650,7 +14650,7 @@
         <v>228</v>
       </c>
       <c r="E596">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F596" t="inlineStr">
         <is>
@@ -14674,7 +14674,7 @@
         <v>229</v>
       </c>
       <c r="E597">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F597" t="inlineStr">
         <is>
@@ -14722,7 +14722,7 @@
         <v>231</v>
       </c>
       <c r="E599">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F599" t="inlineStr">
         <is>
@@ -14818,7 +14818,7 @@
         <v>235</v>
       </c>
       <c r="E603">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F603" t="inlineStr">
         <is>
@@ -14842,7 +14842,7 @@
         <v>236</v>
       </c>
       <c r="E604">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F604" t="inlineStr">
         <is>
@@ -14890,7 +14890,7 @@
         <v>238</v>
       </c>
       <c r="E606">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F606" t="inlineStr">
         <is>
@@ -14962,7 +14962,7 @@
         <v>241</v>
       </c>
       <c r="E609">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F609" t="inlineStr">
         <is>
@@ -15010,7 +15010,7 @@
         <v>243</v>
       </c>
       <c r="E611">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F611" t="inlineStr">
         <is>
@@ -15106,7 +15106,7 @@
         <v>247</v>
       </c>
       <c r="E615">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F615" t="inlineStr">
         <is>
@@ -15130,7 +15130,7 @@
         <v>248</v>
       </c>
       <c r="E616">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F616" t="inlineStr">
         <is>
@@ -15154,7 +15154,7 @@
         <v>249</v>
       </c>
       <c r="E617">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F617" t="inlineStr">
         <is>
@@ -15178,7 +15178,7 @@
         <v>250</v>
       </c>
       <c r="E618">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F618" t="inlineStr">
         <is>
@@ -15202,7 +15202,7 @@
         <v>251</v>
       </c>
       <c r="E619">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F619" t="inlineStr">
         <is>
@@ -15250,7 +15250,7 @@
         <v>253</v>
       </c>
       <c r="E621">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F621" t="inlineStr">
         <is>
@@ -15346,7 +15346,7 @@
         <v>257</v>
       </c>
       <c r="E625">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F625" t="inlineStr">
         <is>
@@ -15394,7 +15394,7 @@
         <v>259</v>
       </c>
       <c r="E627">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F627" t="inlineStr">
         <is>
@@ -15442,7 +15442,7 @@
         <v>261</v>
       </c>
       <c r="E629">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F629" t="inlineStr">
         <is>
@@ -15538,7 +15538,7 @@
         <v>265</v>
       </c>
       <c r="E633">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F633" t="inlineStr">
         <is>
@@ -15562,7 +15562,7 @@
         <v>266</v>
       </c>
       <c r="E634">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F634" t="inlineStr">
         <is>
@@ -15610,7 +15610,7 @@
         <v>268</v>
       </c>
       <c r="E636">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F636" t="inlineStr">
         <is>
@@ -15634,7 +15634,7 @@
         <v>269</v>
       </c>
       <c r="E637">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F637" t="inlineStr">
         <is>
@@ -15706,7 +15706,7 @@
         <v>272</v>
       </c>
       <c r="E640">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F640" t="inlineStr">
         <is>
@@ -15730,7 +15730,7 @@
         <v>273</v>
       </c>
       <c r="E641">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F641" t="inlineStr">
         <is>
@@ -15754,7 +15754,7 @@
         <v>274</v>
       </c>
       <c r="E642">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F642" t="inlineStr">
         <is>
@@ -15778,7 +15778,7 @@
         <v>275</v>
       </c>
       <c r="E643">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F643" t="inlineStr">
         <is>
@@ -15850,7 +15850,7 @@
         <v>278</v>
       </c>
       <c r="E646">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F646" t="inlineStr">
         <is>
@@ -15898,7 +15898,7 @@
         <v>280</v>
       </c>
       <c r="E648">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F648" t="inlineStr">
         <is>
@@ -15946,7 +15946,7 @@
         <v>282</v>
       </c>
       <c r="E650">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F650" t="inlineStr">
         <is>
@@ -15994,7 +15994,7 @@
         <v>284</v>
       </c>
       <c r="E652">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F652" t="inlineStr">
         <is>
@@ -16018,7 +16018,7 @@
         <v>285</v>
       </c>
       <c r="E653">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F653" t="inlineStr">
         <is>
@@ -16090,7 +16090,7 @@
         <v>288</v>
       </c>
       <c r="E656">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F656" t="inlineStr">
         <is>
@@ -16162,7 +16162,7 @@
         <v>291</v>
       </c>
       <c r="E659">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>
@@ -16186,7 +16186,7 @@
         <v>292</v>
       </c>
       <c r="E660">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F660" t="inlineStr">
         <is>
@@ -16234,7 +16234,7 @@
         <v>294</v>
       </c>
       <c r="E662">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F662" t="inlineStr">
         <is>
@@ -16378,7 +16378,7 @@
         <v>300</v>
       </c>
       <c r="E668">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F668" t="inlineStr">
         <is>
@@ -16450,7 +16450,7 @@
         <v>303</v>
       </c>
       <c r="E671">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F671" t="inlineStr">
         <is>
@@ -16522,7 +16522,7 @@
         <v>306</v>
       </c>
       <c r="E674">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F674" t="inlineStr">
         <is>
@@ -16618,7 +16618,7 @@
         <v>310</v>
       </c>
       <c r="E678">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F678" t="inlineStr">
         <is>
@@ -16834,7 +16834,7 @@
         <v>319</v>
       </c>
       <c r="E687">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F687" t="inlineStr">
         <is>
@@ -16882,7 +16882,7 @@
         <v>321</v>
       </c>
       <c r="E689">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F689" t="inlineStr">
         <is>
@@ -16930,7 +16930,7 @@
         <v>323</v>
       </c>
       <c r="E691">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F691" t="inlineStr">
         <is>
@@ -16954,7 +16954,7 @@
         <v>324</v>
       </c>
       <c r="E692">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F692" t="inlineStr">
         <is>
@@ -17050,7 +17050,7 @@
         <v>328</v>
       </c>
       <c r="E696">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F696" t="inlineStr">
         <is>
@@ -17170,7 +17170,7 @@
         <v>333</v>
       </c>
       <c r="E701">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F701" t="inlineStr">
         <is>
@@ -17314,7 +17314,7 @@
         <v>339</v>
       </c>
       <c r="E707">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F707" t="inlineStr">
         <is>
@@ -17386,7 +17386,7 @@
         <v>342</v>
       </c>
       <c r="E710">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F710" t="inlineStr">
         <is>
@@ -17434,7 +17434,7 @@
         <v>344</v>
       </c>
       <c r="E712">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F712" t="inlineStr">
         <is>
@@ -17458,7 +17458,7 @@
         <v>345</v>
       </c>
       <c r="E713">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F713" t="inlineStr">
         <is>
@@ -17578,7 +17578,7 @@
         <v>350</v>
       </c>
       <c r="E718">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F718" t="inlineStr">
         <is>
@@ -17602,7 +17602,7 @@
         <v>351</v>
       </c>
       <c r="E719">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F719" t="inlineStr">
         <is>
@@ -17626,7 +17626,7 @@
         <v>352</v>
       </c>
       <c r="E720">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F720" t="inlineStr">
         <is>
@@ -17650,7 +17650,7 @@
         <v>353</v>
       </c>
       <c r="E721">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F721" t="inlineStr">
         <is>
@@ -17722,7 +17722,7 @@
         <v>356</v>
       </c>
       <c r="E724">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F724" t="inlineStr">
         <is>
@@ -17746,7 +17746,7 @@
         <v>357</v>
       </c>
       <c r="E725">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F725" t="inlineStr">
         <is>
@@ -17818,7 +17818,7 @@
         <v>360</v>
       </c>
       <c r="E728">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F728" t="inlineStr">
         <is>
@@ -17890,7 +17890,7 @@
         <v>363</v>
       </c>
       <c r="E731">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F731" t="inlineStr">
         <is>
@@ -20506,7 +20506,7 @@
         <v>106</v>
       </c>
       <c r="E840">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F840" t="inlineStr">
         <is>
@@ -20530,7 +20530,7 @@
         <v>107</v>
       </c>
       <c r="E841">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F841" t="inlineStr">
         <is>
@@ -20626,7 +20626,7 @@
         <v>111</v>
       </c>
       <c r="E845">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F845" t="inlineStr">
         <is>
@@ -20866,7 +20866,7 @@
         <v>121</v>
       </c>
       <c r="E855">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F855" t="inlineStr">
         <is>
@@ -24154,7 +24154,7 @@
         <v>258</v>
       </c>
       <c r="E992">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F992" t="inlineStr">
         <is>
@@ -24274,7 +24274,7 @@
         <v>263</v>
       </c>
       <c r="E997">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F997" t="inlineStr">
         <is>
@@ -29146,7 +29146,7 @@
         <v>100</v>
       </c>
       <c r="E1200">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1200" t="inlineStr">
         <is>
@@ -31282,7 +31282,7 @@
         <v>189</v>
       </c>
       <c r="E1289">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1289" t="inlineStr">
         <is>
@@ -31570,7 +31570,7 @@
         <v>201</v>
       </c>
       <c r="E1301">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F1301" t="inlineStr">
         <is>
@@ -32698,7 +32698,7 @@
         <v>248</v>
       </c>
       <c r="E1348">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F1348" t="inlineStr">
         <is>
@@ -33514,7 +33514,7 @@
         <v>282</v>
       </c>
       <c r="E1382">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F1382" t="inlineStr">
         <is>
@@ -33826,7 +33826,7 @@
         <v>295</v>
       </c>
       <c r="E1395">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1395" t="inlineStr">
         <is>
@@ -34450,7 +34450,7 @@
         <v>321</v>
       </c>
       <c r="E1421">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F1421" t="inlineStr">
         <is>

</xml_diff>